<commit_message>
excel change in own branch
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffc0462e3503a61e/Desktop/Git practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC104860091964D45ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87B19CE7-55B4-4770-AB1B-10E3EE84F1A2}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC104860091964D45ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C0148E9-859D-4AA6-8D96-18E91834B6D6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -345,15 +351,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>